<commit_message>
backup of the correct code
</commit_message>
<xml_diff>
--- a/testData/test_data.xlsx
+++ b/testData/test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\playwrightTutorial\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\backup\playWrightWebAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>product</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>Sauce Labs Onesie</t>
   </si>
 </sst>
 </file>
@@ -410,7 +407,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added environment specific credentials fetch
</commit_message>
<xml_diff>
--- a/testData/test_data.xlsx
+++ b/testData/test_data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\correctTesDataFile\playWrightWebAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_place_order" sheetId="1" r:id="rId1"/>
     <sheet name="test_place_order1" sheetId="2" r:id="rId2"/>
     <sheet name="test_place_order2" sheetId="3" r:id="rId3"/>
+    <sheet name="test_login_visual" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -554,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -614,4 +615,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated visual tests and test data
</commit_message>
<xml_diff>
--- a/testData/test_data.xlsx
+++ b/testData/test_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\correctTesDataFile\playWrightWebAutomation\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\703360652\playWrightWebAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7EC951-DAFA-43FA-86ED-5CEC6593CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_place_order" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,16 +421,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,7 +464,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -486,16 +487,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,7 +530,7 @@
         <v>3650</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -552,16 +553,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -595,7 +596,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -618,16 +619,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -659,23 +660,6 @@
       </c>
       <c r="E2" s="2">
         <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2">
-        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>